<commit_message>
changed positions of targets in level files to be hittable. put correct angles in the test methods for launching. added a setMethod to set the launcher using integer indexing on the arrayList. Overhauled the physics spreadsheet
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bane/school/semesters/fall_2016/softEng/workspace/FinalProjectCPSW/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="1920" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Theta</t>
   </si>
@@ -46,13 +54,22 @@
   </si>
   <si>
     <t>Y2</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>LauncherX</t>
+  </si>
+  <si>
+    <t>LauncherY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +89,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,9 +126,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -114,6 +140,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -439,162 +470,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="I9" sqref="A9:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f>30/180*PI()</f>
-        <v>0.52359877559829882</v>
+        <v>30</v>
       </c>
       <c r="B2">
+        <f>A2*3.14159265/180</f>
+        <v>0.52359877500000007</v>
+      </c>
+      <c r="C2">
         <v>25</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
       <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
         <v>9.81</v>
       </c>
-      <c r="E2" s="1">
-        <f>B$2*COS(A$2)*C2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <f>B$2*SIN(A$2)*C2-D$2*(C2)^2/2</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <f xml:space="preserve"> 2*B2^2*COS(A2)*SIN(A2)/D2</f>
-        <v>55.174911046409179</v>
-      </c>
       <c r="H2" s="1">
-        <f>B$3*COS(A$3)*C2</f>
-        <v>0</v>
+        <f>$C$2*COS($B2)*$F$2+$D$2</f>
+        <v>18.825317551044851</v>
       </c>
       <c r="I2" s="1">
-        <f>B$3*SIN(A$3)*C2-D$2*C2^2/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <f>C$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>8.023749993523225</v>
+      </c>
+      <c r="J2" s="2">
+        <f xml:space="preserve"> 2*C2^2*COS(B2)*SIN(B2)/G2</f>
+        <v>55.174911008291268</v>
+      </c>
+      <c r="K2" s="1">
+        <f>$C$3*COS($B2)*$F$2+$D$2</f>
+        <v>24.71429029881325</v>
+      </c>
+      <c r="L2" s="1">
+        <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>1.8987499998704644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>57/180*PI()</f>
-        <v>0.99483767363676778</v>
+        <v>57</v>
       </c>
       <c r="B3">
+        <f>A3*3.14159265/180</f>
+        <v>0.9948376725000001</v>
+      </c>
+      <c r="C3">
         <v>38.6</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <f>B$2*COS(A$2)*C3</f>
-        <v>21.650635094610969</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F5" si="0">B$2*SIN(A$2)*C3-D$2*(C3)^2/2</f>
-        <v>7.594999999999998</v>
-      </c>
-      <c r="G3" s="1">
-        <f xml:space="preserve"> 2*B3^2*COS(A3)*SIN(A3)/D2</f>
-        <v>138.75088583783588</v>
-      </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H5" si="1">B$3*COS(A$3)*C3</f>
-        <v>21.02306675158005</v>
+        <f t="shared" ref="H3:H11" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
+        <v>14.807987949605009</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I5" si="2">B$3*SIN(A$3)*C3-D$2*C3^2/2</f>
-        <v>27.467683922693361</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <f>B$2*COS(A$2)*C4</f>
-        <v>43.301270189221938</v>
-      </c>
-      <c r="F4" s="1">
+        <f t="shared" ref="I3:I11" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>12.257132091578699</v>
+      </c>
+      <c r="J3" s="2">
+        <f xml:space="preserve"> 2*C3^2*COS(B3)*SIN(B3)/G2</f>
+        <v>138.75088597828548</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
+        <v>18.511533394190131</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>1.9834176418315739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B10" si="4">A4*3.14159265/180</f>
+        <v>0.17453292500000001</v>
+      </c>
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>5.3799999999999955</v>
-      </c>
-      <c r="H4" s="1">
+        <v>20.310096913085488</v>
+      </c>
+      <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>42.0461335031601</v>
-      </c>
-      <c r="I4" s="1">
+        <v>3.9443522183815904</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>45.12536784538672</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E5" s="1">
-        <f>B$2*COS(A$2)*C5</f>
-        <v>47.631397208144136</v>
-      </c>
-      <c r="F5" s="1">
+        <v>27.006789633803997</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8171620443676317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="4"/>
+        <v>0.34906585000000001</v>
+      </c>
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>3.7597999999999949</v>
-      </c>
-      <c r="H5" s="1">
+        <v>19.746157761529105</v>
+      </c>
+      <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>46.250746853476116</v>
-      </c>
-      <c r="I5" s="1">
+        <v>6.0490017868857171</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>47.479704629925408</v>
+        <v>26.136067583800941</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8592550357377142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="4"/>
+        <v>0.78539816249999994</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>16.838834772764244</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>10.612584756899446</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="2"/>
+        <v>21.64716088914799</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="3"/>
+        <v>1.9505266951379889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="4"/>
+        <v>1.0471975500000001</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>14.250000012953549</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>12.599067539826748</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="2"/>
+        <v>17.650000020000281</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="3"/>
+        <v>1.990256350796535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="4"/>
+        <v>1.3089969375000001</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>11.235238081841269</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>13.847822823774255</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="2"/>
+        <v>12.995207598362919</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="3"/>
+        <v>2.015231456475485</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="4"/>
+        <v>1.3962634</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>10.170602240476942</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>14.083846909189484</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="2"/>
+        <v>11.351409859296396</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="3"/>
+        <v>2.0199519381837896</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="4"/>
+        <v>1.5707963249999999</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>8.0000000224362093</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>14.27375</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="2"/>
+        <v>8.0000000346415074</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="3"/>
+        <v>2.0237499999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>20.5</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7737499999999999</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="2"/>
+        <v>27.3</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7737499999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more overhaul of spreadsheet
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Theta</t>
   </si>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="A9:I9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +481,7 @@
     <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -518,8 +518,11 @@
       <c r="L1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
@@ -551,8 +554,8 @@
         <v>8.023749993523225</v>
       </c>
       <c r="J2" s="2">
-        <f xml:space="preserve"> 2*C2^2*COS(B2)*SIN(B2)/G2</f>
-        <v>55.174911008291268</v>
+        <f xml:space="preserve"> 2*$C$2^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
+        <v>63.174911008291268</v>
       </c>
       <c r="K2" s="1">
         <f>$C$3*COS($B2)*$F$2+$D$2</f>
@@ -562,8 +565,12 @@
         <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
         <v>1.8987499998704644</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="2">
+        <f xml:space="preserve"> 2*$C$3^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
+        <v>139.53345664946187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>57</v>
       </c>
@@ -583,24 +590,28 @@
         <v>12.257132091578699</v>
       </c>
       <c r="J3" s="2">
-        <f xml:space="preserve"> 2*C3^2*COS(B3)*SIN(B3)/G2</f>
-        <v>138.75088597828548</v>
+        <f t="shared" ref="J3:J12" si="2" xml:space="preserve"> 2*$C$2^2*COS($B3)*SIN($B3)/$G$2+$D$2</f>
+        <v>66.20243747243444</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
+        <f t="shared" ref="K3:K11" si="3">$C$3*COS($B3)*$F$2+$D$2</f>
         <v>18.511533394190131</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <f t="shared" ref="L3:L11" si="4">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
         <v>1.9834176418315739</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="2">
+        <f t="shared" ref="M3:M11" si="5" xml:space="preserve"> 2*$C$3^2*COS($B3)*SIN($B3)/$G$2+$D$2</f>
+        <v>146.75088597828548</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B10" si="4">A4*3.14159265/180</f>
+        <f t="shared" ref="B4:B10" si="6">A4*3.14159265/180</f>
         <v>0.17453292500000001</v>
       </c>
       <c r="H4" s="1">
@@ -611,21 +622,29 @@
         <f t="shared" si="1"/>
         <v>3.9443522183815904</v>
       </c>
+      <c r="J4" s="2">
+        <f t="shared" si="2"/>
+        <v>29.790274143148409</v>
+      </c>
       <c r="K4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.006789633803997</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8171620443676317</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="2">
+        <f t="shared" si="5"/>
+        <v>59.94661897972064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
       <c r="B5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.34906585000000001</v>
       </c>
       <c r="H5" s="1">
@@ -636,21 +655,29 @@
         <f t="shared" si="1"/>
         <v>6.0490017868857171</v>
       </c>
+      <c r="J5" s="2">
+        <f t="shared" si="2"/>
+        <v>48.952319640382342</v>
+      </c>
       <c r="K5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26.136067583800941</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8592550357377142</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <f t="shared" si="5"/>
+        <v>105.62770907421452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45</v>
       </c>
       <c r="B6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.78539816249999994</v>
       </c>
       <c r="H6" s="1">
@@ -661,21 +688,29 @@
         <f t="shared" si="1"/>
         <v>10.612584756899446</v>
       </c>
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
+        <v>71.71049949031601</v>
+      </c>
       <c r="K6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21.64716088914799</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9505266951379889</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <f t="shared" si="5"/>
+        <v>159.88175331294599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0471975500000001</v>
       </c>
       <c r="H7" s="1">
@@ -686,21 +721,29 @@
         <f t="shared" si="1"/>
         <v>12.599067539826748</v>
       </c>
+      <c r="J7" s="2">
+        <f t="shared" si="2"/>
+        <v>63.174911122645021</v>
+      </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.650000020000281</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.990256350796535</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <f t="shared" si="5"/>
+        <v>139.53345692207387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>75</v>
       </c>
       <c r="B8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3089969375000001</v>
       </c>
       <c r="H8" s="1">
@@ -711,21 +754,29 @@
         <f t="shared" si="1"/>
         <v>13.847822823774255</v>
       </c>
+      <c r="J8" s="2">
+        <f t="shared" si="2"/>
+        <v>39.855249910213416</v>
+      </c>
       <c r="K8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.995207598362919</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.015231456475485</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <f t="shared" si="5"/>
+        <v>83.940877049954551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
       <c r="B9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3962634</v>
       </c>
       <c r="H9" s="1">
@@ -736,21 +787,29 @@
         <f t="shared" si="1"/>
         <v>14.083846909189484</v>
       </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>29.790274358063169</v>
+      </c>
       <c r="K9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.351409859296396</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0199519381837896</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <f t="shared" si="5"/>
+        <v>59.946619492063675</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
       <c r="B10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5707963249999999</v>
       </c>
       <c r="H10" s="1">
@@ -761,32 +820,33 @@
         <f t="shared" si="1"/>
         <v>14.27375</v>
       </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>8.0000002287075347</v>
+      </c>
       <c r="K10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.0000000346415074</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0237499999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H11" s="1">
-        <f t="shared" si="0"/>
-        <v>20.5</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7737499999999999</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="2"/>
-        <v>27.3</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="3"/>
-        <v>1.7737499999999999</v>
-      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="5"/>
+        <v>8.0000005452241272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Xfinal calculations are shit and don't work
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -473,7 +473,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,18 +540,18 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>9.81</v>
       </c>
       <c r="H2" s="1">
         <f>$C$2*COS($B2)*$F$2+$D$2</f>
-        <v>18.825317551044851</v>
+        <v>51.301270204179403</v>
       </c>
       <c r="I2" s="1">
         <f>C$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>8.023749993523225</v>
+        <v>8.3799999740929003</v>
       </c>
       <c r="J2" s="2">
         <f xml:space="preserve"> 2*$C$2^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -559,11 +559,11 @@
       </c>
       <c r="K2" s="1">
         <f>$C$3*COS($B2)*$F$2+$D$2</f>
-        <v>24.71429029881325</v>
+        <v>74.857161195252999</v>
       </c>
       <c r="L2" s="1">
         <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>1.8987499998704644</v>
+        <v>-14.620000002072569</v>
       </c>
       <c r="M2" s="2">
         <f xml:space="preserve"> 2*$C$3^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -583,259 +583,211 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H11" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
-        <v>14.807987949605009</v>
+        <v>35.231951798420035</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I11" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>12.257132091578699</v>
-      </c>
-      <c r="J3" s="2">
-        <f t="shared" ref="J3:J12" si="2" xml:space="preserve"> 2*$C$2^2*COS($B3)*SIN($B3)/$G$2+$D$2</f>
-        <v>66.20243747243444</v>
-      </c>
+        <v>25.313528366314795</v>
+      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K11" si="3">$C$3*COS($B3)*$F$2+$D$2</f>
-        <v>18.511533394190131</v>
+        <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
+        <v>50.046133576760532</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L11" si="4">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>1.9834176418315739</v>
-      </c>
-      <c r="M3" s="2">
-        <f t="shared" ref="M3:M11" si="5" xml:space="preserve"> 2*$C$3^2*COS($B3)*SIN($B3)/$G$2+$D$2</f>
-        <v>146.75088597828548</v>
-      </c>
+        <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>-13.265317730694818</v>
+      </c>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B10" si="6">A4*3.14159265/180</f>
+        <f t="shared" ref="B4:B10" si="4">A4*3.14159265/180</f>
         <v>0.17453292500000001</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>20.310096913085488</v>
+        <v>57.240387652341958</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>3.9443522183815904</v>
-      </c>
-      <c r="J4" s="2">
+        <v>-7.9375911264736381</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>29.790274143148409</v>
-      </c>
-      <c r="K4" s="1">
+        <v>84.027158535215989</v>
+      </c>
+      <c r="L4" s="1">
         <f t="shared" si="3"/>
-        <v>27.006789633803997</v>
-      </c>
-      <c r="L4" s="1">
-        <f t="shared" si="4"/>
-        <v>1.8171620443676317</v>
-      </c>
-      <c r="M4" s="2">
-        <f t="shared" si="5"/>
-        <v>59.94661897972064</v>
-      </c>
+        <v>-15.925407290117892</v>
+      </c>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
       <c r="B5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.34906585000000001</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>19.746157761529105</v>
+        <v>54.984631046116426</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>6.0490017868857171</v>
-      </c>
-      <c r="J5" s="2">
+        <v>0.48100714754286855</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>48.952319640382342</v>
-      </c>
-      <c r="K5" s="1">
+        <v>80.544270335203763</v>
+      </c>
+      <c r="L5" s="1">
         <f t="shared" si="3"/>
-        <v>26.136067583800941</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" si="4"/>
-        <v>1.8592550357377142</v>
-      </c>
-      <c r="M5" s="2">
-        <f t="shared" si="5"/>
-        <v>105.62770907421452</v>
-      </c>
+        <v>-15.251919428196572</v>
+      </c>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45</v>
       </c>
       <c r="B6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.78539816249999994</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>16.838834772764244</v>
+        <v>43.355339091056969</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>10.612584756899446</v>
-      </c>
-      <c r="J6" s="2">
+        <v>18.735339027597785</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>71.71049949031601</v>
-      </c>
-      <c r="K6" s="1">
+        <v>62.588643556591961</v>
+      </c>
+      <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>21.64716088914799</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="4"/>
-        <v>1.9505266951379889</v>
-      </c>
-      <c r="M6" s="2">
-        <f t="shared" si="5"/>
-        <v>159.88175331294599</v>
-      </c>
+        <v>-13.791572877792177</v>
+      </c>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0471975500000001</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>14.250000012953549</v>
+        <v>33.000000051814197</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>12.599067539826748</v>
-      </c>
-      <c r="J7" s="2">
+        <v>26.681270159306994</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>63.174911122645021</v>
-      </c>
-      <c r="K7" s="1">
+        <v>46.600000080001124</v>
+      </c>
+      <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>17.650000020000281</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="4"/>
-        <v>1.990256350796535</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="5"/>
-        <v>139.53345692207387</v>
-      </c>
+        <v>-13.155898387255441</v>
+      </c>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>75</v>
       </c>
       <c r="B8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3089969375000001</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>11.235238081841269</v>
+        <v>20.940952327365075</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>13.847822823774255</v>
-      </c>
-      <c r="J8" s="2">
+        <v>31.67629129509702</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>39.855249910213416</v>
-      </c>
-      <c r="K8" s="1">
+        <v>27.980830393451676</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>12.995207598362919</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="4"/>
-        <v>2.015231456475485</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="5"/>
-        <v>83.940877049954551</v>
-      </c>
+        <v>-12.756296696392239</v>
+      </c>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
       <c r="B9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3962634</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>10.170602240476942</v>
+        <v>16.682408961907765</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>14.083846909189484</v>
-      </c>
-      <c r="J9" s="2">
+        <v>32.62038763675794</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>29.790274358063169</v>
-      </c>
-      <c r="K9" s="1">
+        <v>21.405639437185588</v>
+      </c>
+      <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>11.351409859296396</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="4"/>
-        <v>2.0199519381837896</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="5"/>
-        <v>59.946619492063675</v>
-      </c>
+        <v>-12.680768989059366</v>
+      </c>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
       <c r="B10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.5707963249999999</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>8.0000000224362093</v>
+        <v>8.0000000897448373</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>14.27375</v>
-      </c>
-      <c r="J10" s="2">
+        <v>33.379999999999995</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>8.0000002287075347</v>
-      </c>
-      <c r="K10" s="1">
+        <v>8.000000138566028</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="3"/>
-        <v>8.0000000346415074</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="4"/>
-        <v>2.0237499999999997</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="5"/>
-        <v>8.0000005452241272</v>
-      </c>
+        <v>-12.620000000000001</v>
+      </c>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H11" s="1"/>

</xml_diff>

<commit_message>
changed the velocities of the launchers
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -473,7 +473,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,7 @@
       </c>
       <c r="K2" s="1">
         <f>$C$3*COS($B2)*$F$2+$D$2</f>
-        <v>74.857161195252999</v>
+        <v>73.817930710352698</v>
       </c>
       <c r="L2" s="1">
         <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
@@ -567,7 +567,7 @@
       </c>
       <c r="M2" s="2">
         <f xml:space="preserve"> 2*$C$3^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
-        <v>139.53345664946187</v>
+        <v>135.47611439355614</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -579,23 +579,23 @@
         <v>0.9948376725000001</v>
       </c>
       <c r="C3">
-        <v>38.6</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H11" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
+        <f t="shared" ref="H3:H10" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
         <v>35.231951798420035</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I11" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <f t="shared" ref="I3:I10" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
         <v>25.313528366314795</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
-        <v>50.046133576760532</v>
+        <f t="shared" ref="K3:K10" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
+        <v>49.39256673359845</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <f t="shared" ref="L3:L10" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
         <v>-13.265317730694818</v>
       </c>
       <c r="M3" s="2"/>
@@ -619,7 +619,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>84.027158535215989</v>
+        <v>82.845389231559778</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="3"/>
@@ -646,7 +646,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>80.544270335203763</v>
+        <v>79.416639190096973</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="3"/>
@@ -673,7 +673,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>62.588643556591961</v>
+        <v>61.740115418406596</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
@@ -700,7 +700,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>46.600000080001124</v>
+        <v>46.00000007875758</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
@@ -727,7 +727,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>27.980830393451676</v>
+        <v>27.670247537594911</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
@@ -754,7 +754,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>21.405639437185588</v>
+        <v>21.197261622099802</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
@@ -781,7 +781,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>8.000000138566028</v>
+        <v>8.0000001364121527</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
added another angle to evaluate
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1920" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="1960" windowWidth="19040" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,18 +540,18 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="G2">
         <v>9.81</v>
       </c>
       <c r="H2" s="1">
         <f>$C$2*COS($B2)*$F$2+$D$2</f>
-        <v>51.301270204179403</v>
+        <v>23.155444571462787</v>
       </c>
       <c r="I2" s="1">
         <f>C$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>8.3799999740929003</v>
+        <v>9.346549990932516</v>
       </c>
       <c r="J2" s="2">
         <f xml:space="preserve"> 2*$C$2^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -559,11 +559,11 @@
       </c>
       <c r="K2" s="1">
         <f>$C$3*COS($B2)*$F$2+$D$2</f>
-        <v>73.817930710352698</v>
+        <v>31.036275748623442</v>
       </c>
       <c r="L2" s="1">
         <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>-14.620000002072569</v>
+        <v>0.84154999974611044</v>
       </c>
       <c r="M2" s="2">
         <f xml:space="preserve"> 2*$C$3^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -582,21 +582,21 @@
         <v>38</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H10" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
-        <v>35.231951798420035</v>
+        <f t="shared" ref="H3:H11" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
+        <v>17.531183129447012</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I10" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>25.313528366314795</v>
+        <f t="shared" ref="I3:I11" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>15.273284928210177</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K10" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
-        <v>49.39256673359845</v>
+        <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
+        <v>22.487398356759456</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L10" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>-13.265317730694818</v>
+        <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>1.0074985779898851</v>
       </c>
       <c r="M3" s="2"/>
     </row>
@@ -605,25 +605,25 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B10" si="4">A4*3.14159265/180</f>
+        <f t="shared" ref="B4:B11" si="4">A4*3.14159265/180</f>
         <v>0.17453292500000001</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>57.240387652341958</v>
+        <v>25.234135678319685</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>-7.9375911264736381</v>
+        <v>3.6353931057342268</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>82.845389231559778</v>
+        <v>34.195886231045918</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="3"/>
-        <v>-15.925407290117892</v>
+        <v>0.68163760696055853</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -637,20 +637,20 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>54.984631046116426</v>
+        <v>24.444620866140749</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>0.48100714754286855</v>
+        <v>6.5819025016400037</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>79.416639190096973</v>
+        <v>32.995823716533934</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="3"/>
-        <v>-15.251919428196572</v>
+        <v>0.76413987004592032</v>
       </c>
       <c r="M5" s="2"/>
     </row>
@@ -664,20 +664,20 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>43.355339091056969</v>
+        <v>20.374368681869939</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>18.735339027597785</v>
+        <v>12.970918659659224</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>61.740115418406596</v>
+        <v>26.809040396442306</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>-13.791572877792177</v>
+        <v>0.94303232247045843</v>
       </c>
       <c r="M6" s="2"/>
     </row>
@@ -691,114 +691,141 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>33.000000051814197</v>
+        <v>16.750000018134969</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>26.681270159306994</v>
+        <v>15.751994555757447</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>46.00000007875758</v>
+        <v>21.300000027565154</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>-13.155898387255441</v>
+        <v>1.0209024475612085</v>
       </c>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>1.3089969375000001</v>
+        <v>1.1344640125000001</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>20.940952327365075</v>
+        <v>15.395819601022282</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>31.67629129509702</v>
+        <v>16.45693626355407</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>27.670247537594911</v>
+        <v>19.241645793553872</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-12.756296696392239</v>
+        <v>1.0406408153795139</v>
       </c>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B9">
         <f t="shared" si="4"/>
-        <v>1.3962634</v>
+        <v>1.3089969375000001</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>16.682408961907765</v>
+        <v>12.529333314577777</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>32.62038763675794</v>
+        <v>17.500251953283957</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>21.197261622099802</v>
+        <v>14.884586638158218</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>-12.680768989059366</v>
+        <v>1.0698536546919508</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B10">
         <f t="shared" si="4"/>
-        <v>1.5707963249999999</v>
+        <v>1.3962634</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>8.0000000897448373</v>
+        <v>11.038843136667717</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>33.379999999999995</v>
+        <v>17.830685672865279</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>8.0000001364121527</v>
+        <v>12.61904156773493</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="3"/>
-        <v>-12.620000000000001</v>
+        <v>1.0791057988402279</v>
       </c>
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="4"/>
+        <v>1.5707963249999999</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>8.0000000314106927</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>18.096550000000001</v>
+      </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="K11" s="1">
+        <f t="shared" si="2"/>
+        <v>8.000000047744253</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0865500000000001</v>
+      </c>
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="2"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added the slow trebuchet to calculations
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="1960" windowWidth="19040" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="1960" windowWidth="27060" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Theta</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Gravity</t>
   </si>
   <si>
-    <t>Xf</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -63,6 +60,18 @@
   </si>
   <si>
     <t>LauncherY</t>
+  </si>
+  <si>
+    <t>Xf1</t>
+  </si>
+  <si>
+    <t>Xf2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>Y3</t>
   </si>
 </sst>
 </file>
@@ -470,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="O2" sqref="O2:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,9 +490,9 @@
     <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -492,10 +501,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -504,25 +513,31 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
       <c r="M1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
@@ -540,18 +555,18 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="G2">
         <v>9.81</v>
       </c>
       <c r="H2" s="1">
         <f>$C$2*COS($B2)*$F$2+$D$2</f>
-        <v>23.155444571462787</v>
+        <v>26.403039836776244</v>
       </c>
       <c r="I2" s="1">
-        <f>C$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>9.346549990932516</v>
+        <f>$C$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>10.081137488989484</v>
       </c>
       <c r="J2" s="2">
         <f xml:space="preserve"> 2*$C$2^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -559,18 +574,26 @@
       </c>
       <c r="K2" s="1">
         <f>$C$3*COS($B2)*$F$2+$D$2</f>
-        <v>31.036275748623442</v>
+        <v>35.972620551899894</v>
       </c>
       <c r="L2" s="1">
         <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>0.84154999974611044</v>
+        <v>-0.18261250037435772</v>
       </c>
       <c r="M2" s="2">
         <f xml:space="preserve"> 2*$C$3^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
         <v>135.47611439355614</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="1">
+        <f>$C$4*COS($B2)*$F$2+$D$2</f>
+        <v>15.361215934710497</v>
+      </c>
+      <c r="O2" s="1">
+        <f>$C$4*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>3.7061374955957933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>57</v>
       </c>
@@ -583,240 +606,315 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H11" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
-        <v>17.531183129447012</v>
+        <v>19.573579514328515</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I11" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>15.273284928210177</v>
+        <v>17.277887055683788</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
-        <v>22.487398356759456</v>
+        <v>25.591840861779342</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>1.0074985779898851</v>
+        <v>6.2076984893248977E-2</v>
       </c>
       <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N11" si="4">$C$4*COS($B3)*$F$2+$D$2</f>
+        <v>12.629431805731407</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O11" si="5">$C$4*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
+        <v>6.5848373222735148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B11" si="4">A4*3.14159265/180</f>
+        <f t="shared" ref="B4:B11" si="6">A4*3.14159265/180</f>
         <v>0.17453292500000001</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>25.234135678319685</v>
+        <v>28.927164752245332</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>3.6353931057342268</v>
+        <v>3.1461612712487041</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>34.195886231045918</v>
+        <v>39.809290423412904</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="3"/>
-        <v>0.68163760696055853</v>
+        <v>-0.41840169177754394</v>
       </c>
       <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="1">
+        <f t="shared" si="4"/>
+        <v>16.370865900898131</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="5"/>
+        <v>0.93214700849948162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
       <c r="B5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.34906585000000001</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>24.444620866140749</v>
+        <v>27.968468194599481</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>6.5819025016400037</v>
+        <v>6.7240655377057195</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>32.995823716533934</v>
+        <v>38.352071655791214</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="3"/>
-        <v>0.76413987004592032</v>
+        <v>-0.29675294671800545</v>
       </c>
       <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1">
+        <f t="shared" si="4"/>
+        <v>15.987387277839792</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="5"/>
+        <v>2.3633087150822876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45</v>
       </c>
       <c r="B6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.78539816249999994</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>20.374368681869939</v>
+        <v>23.026019113699213</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>12.970918659659224</v>
+        <v>14.48215658672906</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>26.809040396442306</v>
+        <v>30.839549052822804</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>0.94303232247045843</v>
+        <v>-3.2977851051211982E-2</v>
       </c>
       <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>14.010407645479685</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="5"/>
+        <v>5.466545134691625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0471975500000001</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>16.750000018134969</v>
+        <v>18.625000022021034</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>15.751994555757447</v>
+        <v>17.859177317705473</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>21.300000027565154</v>
+        <v>24.150000033471972</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>1.0209024475612085</v>
+        <v>8.1840853801986135E-2</v>
       </c>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="1">
+        <f t="shared" si="4"/>
+        <v>12.250000008808414</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="5"/>
+        <v>6.8173534270821889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>65</v>
       </c>
       <c r="B8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1344640125000001</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>15.395819601022282</v>
+        <v>16.980638086955629</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>16.45693626355407</v>
+        <v>18.715177962887083</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>19.241645793553872</v>
+        <v>21.650569892172555</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>1.0406408153795139</v>
+        <v>0.11094487573816103</v>
       </c>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="1">
+        <f t="shared" si="4"/>
+        <v>11.592255234782252</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="5"/>
+        <v>7.1597536851548345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>75</v>
       </c>
       <c r="B9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3089969375000001</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>12.529333314577777</v>
+        <v>13.499904739130157</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>17.500251953283957</v>
+        <v>19.982061300416234</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>14.884586638158218</v>
+        <v>16.359855203477835</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>1.0698536546919508</v>
+        <v>0.15401890921415218</v>
       </c>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="1">
+        <f t="shared" si="4"/>
+        <v>10.199961895652063</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="5"/>
+        <v>7.6665070201664935</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>80</v>
       </c>
       <c r="B10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3962634</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>11.038843136667717</v>
+        <v>11.6900238088108</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>17.830685672865279</v>
+        <v>20.383302245622122</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>12.61904156773493</v>
+        <v>13.608836189392417</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="3"/>
-        <v>1.0791057988402279</v>
+        <v>0.1676611013511522</v>
       </c>
       <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="1">
+        <f t="shared" si="4"/>
+        <v>9.4760095235243202</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="5"/>
+        <v>7.8270033982488503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>90</v>
       </c>
       <c r="B11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5707963249999999</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
-        <v>8.0000000314106927</v>
+        <v>8.0000000381415557</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>18.096550000000001</v>
+        <v>20.706137500000001</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1">
         <f t="shared" si="2"/>
-        <v>8.000000047744253</v>
+        <v>8.0000000579751642</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="3"/>
-        <v>1.0865500000000001</v>
+        <v>0.17863749999999978</v>
       </c>
       <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="1">
+        <f t="shared" si="4"/>
+        <v>8.0000000152566226</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="5"/>
+        <v>7.9561375000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
@@ -824,7 +922,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J13" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
playing with physics calcs
</commit_message>
<xml_diff>
--- a/Final Project Parabolic Calculations.xlsx
+++ b/Final Project Parabolic Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="1960" windowWidth="27060" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="2400" yWindow="2100" windowWidth="27060" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,18 +555,18 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>0.85</v>
+        <v>1.5</v>
       </c>
       <c r="G2">
         <v>9.81</v>
       </c>
       <c r="H2" s="1">
         <f>$C$2*COS($B2)*$F$2+$D$2</f>
-        <v>26.403039836776244</v>
+        <v>40.475952653134556</v>
       </c>
       <c r="I2" s="1">
         <f>$C$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>10.081137488989484</v>
+        <v>10.713749980569675</v>
       </c>
       <c r="J2" s="2">
         <f xml:space="preserve"> 2*$C$2^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -574,11 +574,11 @@
       </c>
       <c r="K2" s="1">
         <f>$C$3*COS($B2)*$F$2+$D$2</f>
-        <v>35.972620551899894</v>
+        <v>57.363448032764524</v>
       </c>
       <c r="L2" s="1">
         <f>F$2*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>-0.18261250037435772</v>
+        <v>-6.9112500011658202</v>
       </c>
       <c r="M2" s="2">
         <f xml:space="preserve"> 2*$C$3^2*COS($B2)*SIN($B2)/$G$2+$D$2</f>
@@ -586,11 +586,11 @@
       </c>
       <c r="N2" s="1">
         <f>$C$4*COS($B2)*$F$2+$D$2</f>
-        <v>15.361215934710497</v>
+        <v>20.990381061253821</v>
       </c>
       <c r="O2" s="1">
         <f>$C$4*SIN($B2)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>3.7061374955957933</v>
+        <v>-0.53625000777213039</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -606,29 +606,29 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H11" si="0">$C$2*COS($B3)*$F$2+$D$2</f>
-        <v>19.573579514328515</v>
+        <v>28.423963848815028</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I11" si="1">C$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>17.277887055683788</v>
+        <v>23.413896274736096</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K11" si="2">$C$3*COS($B3)*$F$2+$D$2</f>
-        <v>25.591840861779342</v>
+        <v>39.044425050198839</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L11" si="3">F$2*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>6.2076984893248977E-2</v>
+        <v>-6.1492412235158351</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N11" si="4">$C$4*COS($B3)*$F$2+$D$2</f>
-        <v>12.629431805731407</v>
+        <v>16.169585539526011</v>
       </c>
       <c r="O3" s="1">
         <f t="shared" ref="O3:O11" si="5">$C$4*SIN($B3)*$F$2-$G$2*($F$2)^2/2+$E$2</f>
-        <v>6.5848373222735148</v>
+        <v>4.5438085098944381</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -644,29 +644,29 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>28.927164752245332</v>
+        <v>44.930290739256471</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>3.1461612712487041</v>
+        <v>-1.5244433448552286</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
-        <v>39.809290423412904</v>
+        <v>64.134041923669827</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="3"/>
-        <v>-0.41840169177754394</v>
+        <v>-7.6455416006913151</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="1">
         <f t="shared" si="4"/>
-        <v>16.370865900898131</v>
+        <v>22.772116295702588</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" si="5"/>
-        <v>0.93214700849948162</v>
+        <v>-5.431527337942093</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -679,29 +679,29 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>27.968468194599481</v>
+        <v>43.238473284587322</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>6.7240655377057195</v>
+        <v>4.7895053606571505</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>38.352071655791214</v>
+        <v>61.562479392572726</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="3"/>
-        <v>-0.29675294671800545</v>
+        <v>-7.266704678360572</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="1">
         <f t="shared" si="4"/>
-        <v>15.987387277839792</v>
+        <v>22.095389313834929</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
-        <v>2.3633087150822876</v>
+        <v>-2.9059478557371401</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -714,29 +714,29 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>23.026019113699213</v>
+        <v>34.516504318292725</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>14.48215658672906</v>
+        <v>18.480254270698339</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>30.839549052822804</v>
+        <v>48.305086563804949</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>-3.2977851051211982E-2</v>
+        <v>-6.4452597437581005</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="1">
         <f t="shared" si="4"/>
-        <v>14.010407645479685</v>
+        <v>18.606601727317091</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="5"/>
-        <v>5.466545134691625</v>
+        <v>2.5703517082793361</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -749,29 +749,29 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>18.625000022021034</v>
+        <v>26.750000038860648</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>17.859177317705473</v>
+        <v>24.439702619480244</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>24.150000033471972</v>
+        <v>36.500000059068185</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>8.1840853801986135E-2</v>
+        <v>-6.0876928428311867</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="1">
         <f t="shared" si="4"/>
-        <v>12.250000008808414</v>
+        <v>15.500000015544259</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="5"/>
-        <v>6.8173534270821889</v>
+        <v>4.9541310477920977</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -784,29 +784,29 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>16.980638086955629</v>
+        <v>23.848184859333465</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>18.715177962887083</v>
+        <v>25.950291993330147</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>21.650569892172555</v>
+        <v>32.089240986186866</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>0.11094487573816103</v>
+        <v>-5.9970574804001924</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="1">
         <f t="shared" si="4"/>
-        <v>11.592255234782252</v>
+        <v>14.339273943733385</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" si="5"/>
-        <v>7.1597536851548345</v>
+        <v>5.5583667973320594</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -819,29 +819,29 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>13.499904739130157</v>
+        <v>17.705714245523808</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>19.982061300416234</v>
+        <v>28.185968471322759</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>16.359855203477835</v>
+        <v>22.752685653196181</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>0.15401890921415218</v>
+        <v>-5.8629168917206353</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="1">
         <f t="shared" si="4"/>
-        <v>10.199961895652063</v>
+        <v>11.882285698209522</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="5"/>
-        <v>7.6665070201664935</v>
+        <v>6.4526373885291068</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -854,29 +854,29 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>11.6900238088108</v>
+        <v>14.511806721430823</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>20.383302245622122</v>
+        <v>28.894040727568452</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>13.608836189392417</v>
+        <v>17.897946216574852</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="3"/>
-        <v>0.1676611013511522</v>
+        <v>-5.8204325563458941</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="1">
         <f t="shared" si="4"/>
-        <v>9.4760095235243202</v>
+        <v>10.604722688572329</v>
       </c>
       <c r="O10" s="1">
         <f t="shared" si="5"/>
-        <v>7.8270033982488503</v>
+        <v>6.7358662910273814</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -889,29 +889,29 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
-        <v>8.0000000381415557</v>
+        <v>8.000000067308628</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>20.706137500000001</v>
+        <v>29.463749999999997</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1">
         <f t="shared" si="2"/>
-        <v>8.0000000579751642</v>
+        <v>8.0000001023091141</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="3"/>
-        <v>0.17863749999999978</v>
+        <v>-5.7862500000000008</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="1">
         <f t="shared" si="4"/>
-        <v>8.0000000152566226</v>
+        <v>8.0000000269234519</v>
       </c>
       <c r="O11" s="1">
         <f t="shared" si="5"/>
-        <v>7.9561375000000005</v>
+        <v>6.9637499999999992</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>